<commit_message>
Criação do arquivo 'pca_img.py'
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reitoriaunespbr-my.sharepoint.com/personal/luiz_h_santos_unesp_br/Documents/TCC/Projeto Cientifico 2/Datasets/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reitoriaunespbr-my.sharepoint.com/personal/luiz_h_santos_unesp_br/Documents/TCC/Projeto Cientifico 2/Datasets/PC2_scripts/PC2_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_AD4D361C20488DEA4E38A025741E677E5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D237E6B0-8A37-4075-A81B-8EA9E44BFFC8}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_AD4D361C20488DEA4E38A025741E677E5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E602A7C-7F74-4837-9817-DA490A03DBE8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Sigla</t>
   </si>
@@ -81,9 +92,6 @@
     <t>SENTIMENT</t>
   </si>
   <si>
-    <t>SMS</t>
-  </si>
-  <si>
     <t>SPAMBASE</t>
   </si>
   <si>
@@ -115,6 +123,12 @@
   </si>
   <si>
     <t>https://www.kaggle.com/datasets/uciml/sms-spam-collection-dataset</t>
+  </si>
+  <si>
+    <t>SMS-SPAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/t-davidson/hate-speech-and-offensive-language/tree/master/data </t>
   </si>
 </sst>
 </file>
@@ -492,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,7 +515,7 @@
     <col min="1" max="1" width="19" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="65.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="79.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="65.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -513,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -527,10 +541,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -538,13 +552,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -552,13 +566,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -566,13 +580,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -580,10 +594,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -591,10 +605,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -602,7 +616,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -615,7 +629,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -633,7 +653,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -646,34 +666,34 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -683,8 +703,9 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{CF0E4DAA-6CFF-41E5-9277-C3435E1718D7}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{A34267EE-2740-40D7-96D9-FBE1FD1F5A06}"/>
     <hyperlink ref="D16" r:id="rId5" xr:uid="{789C1340-4C6C-45AA-B894-B60FAC5CAD36}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{C3401999-768F-4350-A430-1CC7783752CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tentativas de abrir o conjunto de dados 'sms spam'
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reitoriaunespbr-my.sharepoint.com/personal/luiz_h_santos_unesp_br/Documents/TCC/Projeto Cientifico 2/Datasets/PC2_scripts/PC2_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_AD4D361C20488DEA4E38A025741E677E5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E602A7C-7F74-4837-9817-DA490A03DBE8}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="11_AD4D361C20488DEA4E38A025741E677E5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55126E3E-5DE2-48B5-A45E-299364D791CA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>